<commit_message>
refactored duplcate codes and applied custom indexed colors to border colors(task #35)
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/wrong_color.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/wrong_color.xlsx
@@ -51,7 +51,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -64,8 +64,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -82,17 +88,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="61"/>
+      </left>
+      <right style="thin">
+        <color indexed="61"/>
+      </right>
+      <top style="thin">
+        <color indexed="61"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="61"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -167,6 +190,7 @@
       <rgbColor rgb="00000000"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFE8E8E8"/>
       <color rgb="FF5A97FF"/>
       <color rgb="FF003366"/>
     </mruColors>
@@ -497,7 +521,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -516,12 +540,14 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
+      <c r="A2" s="4"/>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>

</xml_diff>